<commit_message>
feat: atualizando os tests
</commit_message>
<xml_diff>
--- a/agro-mvc/tests/Controle_de_Treinamentos.xlsx
+++ b/agro-mvc/tests/Controle_de_Treinamentos.xlsx
@@ -22,16 +22,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="99">
   <si>
-    <t xml:space="preserve">Funcionário</t>
+    <t xml:space="preserve">Nome</t>
   </si>
   <si>
     <t xml:space="preserve">Profissão</t>
   </si>
   <si>
-    <t xml:space="preserve">Treinamento Requerido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Status Treinamento</t>
+    <t xml:space="preserve">Treinamento Obrigatório</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Situação de Treinamento</t>
   </si>
   <si>
     <t xml:space="preserve">Data de Vencimento</t>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Completo</t>
   </si>
   <si>
-    <t xml:space="preserve">23/07/2026</t>
+    <t xml:space="preserve">15/12/2030</t>
   </si>
   <si>
     <t xml:space="preserve">Gestao de Residuos Industriais</t>
@@ -323,8 +323,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -406,13 +407,21 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -610,1069 +619,1069 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="38.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.77"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="D27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="0" t="s">
+      <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="D28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D29" s="0" t="s">
+      <c r="D29" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="0" t="s">
+      <c r="D30" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="0" t="s">
+      <c r="D33" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="0" t="s">
+      <c r="D34" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D36" s="0" t="s">
+      <c r="D36" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D38" s="0" t="s">
+      <c r="D38" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D39" s="0" t="s">
+      <c r="D39" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D40" s="0" t="s">
+      <c r="D40" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="D41" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D42" s="0" t="s">
+      <c r="D42" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="0" t="s">
+      <c r="D43" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="0" t="s">
+      <c r="D44" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D45" s="0" t="s">
+      <c r="D45" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="0" t="s">
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="D47" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D48" s="0" t="s">
+      <c r="D48" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="0" t="s">
+      <c r="D49" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="0" t="s">
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="0" t="s">
+      <c r="D51" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D52" s="0" t="s">
+      <c r="D52" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="0" t="s">
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="0" t="s">
+      <c r="D54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D55" s="0" t="s">
+      <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E56" s="0" t="s">
+      <c r="D56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="0" t="s">
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D58" s="0" t="s">
+      <c r="D58" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E59" s="0" t="s">
+      <c r="D59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D60" s="0" t="s">
+      <c r="D60" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D61" s="0" t="s">
+      <c r="D61" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D62" s="0" t="s">
+      <c r="D62" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="0" t="s">
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B64" s="0" t="s">
+      <c r="B64" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="0" t="s">
+      <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E65" s="0" t="s">
+      <c r="D65" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D66" s="0" t="s">
+      <c r="D66" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="0" t="s">
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+      <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D68" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="0" t="s">
+      <c r="D68" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" s="1" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Melhorando OOP da projeto. Apartir daqui fazer as coisas desse jeito
</commit_message>
<xml_diff>
--- a/agro-mvc/tests/Controle_de_Treinamentos.xlsx
+++ b/agro-mvc/tests/Controle_de_Treinamentos.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="98">
   <si>
     <t xml:space="preserve">Nome</t>
   </si>
@@ -49,13 +49,10 @@
     <t xml:space="preserve">Completo</t>
   </si>
   <si>
-    <t xml:space="preserve">15/12/2030</t>
+    <t xml:space="preserve">22/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">Gestao de Residuos Industriais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/01/2025</t>
   </si>
   <si>
     <t xml:space="preserve">Logistica de Producao</t>
@@ -619,7 +616,7 @@
   <dimension ref="A1:E68"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -679,7 +676,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -690,193 +687,193 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C15" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>7</v>
@@ -885,164 +882,164 @@
         <v>8</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C24" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C25" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C26" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
@@ -1051,212 +1048,212 @@
         <v>8</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="C34" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="C35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="D36" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>60</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>10</v>
@@ -1265,424 +1262,424 @@
         <v>8</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="D43" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C44" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C46" s="1" t="s">
+      <c r="D46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B47" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C47" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C48" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="C50" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B52" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C52" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C54" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C55" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B56" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B56" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="C56" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="C57" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="D57" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B58" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B58" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C58" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B59" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="C59" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B60" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B60" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C60" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>91</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="C63" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C64" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>93</v>
-      </c>
       <c r="C65" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B66" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C66" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B67" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="C67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="C68" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Passando as configuracoes do banco e os sql para .env e utilizando define para exporta-los para o codigo
</commit_message>
<xml_diff>
--- a/agro-mvc/tests/Controle_de_Treinamentos.xlsx
+++ b/agro-mvc/tests/Controle_de_Treinamentos.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,311 +19,313 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="98">
-  <si>
-    <t xml:space="preserve">Nome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Profissão</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Treinamento Obrigatório</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Situação de Treinamento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data de Vencimento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amanda Duarte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Conferente de Estoque</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestao de Fornecedores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/01/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestao de Residuos Industriais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logistica de Producao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pendente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ana Costa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supervisor de Producao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestao de Equipes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/11/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gestao de Projetos Industriais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seguranca Quimica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatriz Castro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coordenador de Seguranca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Primeiros Socorros Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seguranca em Maquinas Industriais</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/07/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bruno Carvalho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supervisor de Qualidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auditoria Interna de Qualidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de Qualidade em Alimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05/10/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Legislacao Sanitaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/07/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camila Ribeiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerente de Producao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09/04/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos Souza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engenheiro de Alimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISO 22000 - Seguranca de Alimentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20/06/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnologia de Processamento de Frutas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diego Fernandes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operador de Caldeira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manutencao Preventiva Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fernanda Lima</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Responsavel Tecnico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26/06/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gustavo Nunes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutricionista Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04/01/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabela Freitas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Assistente de RH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/02/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Joao Silva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operador de Maquinas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Boas Praticas de Fabricacao (BPF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07/08/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juliana Alves</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Encarregado de Logistica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/07/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laura Martins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eletricista Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eletricidade Industrial Basica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lucas Santos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analista de Qualidade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analise Microbiologica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/11/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19/12/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Calibracao de Equipamentos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marcos Torres</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auxiliar de Producao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21/12/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Higienizacao Industrial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maria Oliveira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnico de Laboratorio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16/10/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25/08/2027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29/01/2026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patricia Mendes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operador de Processos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operacao de Empacotamento Automatizado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02/03/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18/12/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pedro Rocha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auxiliar de Limpeza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rafael Pereira</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnico de Manutencao</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17/11/2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28/03/2025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thiago Gomes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Operador de Empacotamento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27/11/2025</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="99">
+  <si>
+    <t>Nome</t>
+  </si>
+  <si>
+    <t>Profissão</t>
+  </si>
+  <si>
+    <t>Treinamento Obrigatório</t>
+  </si>
+  <si>
+    <t>Situação de Treinamento</t>
+  </si>
+  <si>
+    <t>Data de Vencimento</t>
+  </si>
+  <si>
+    <t>Amanda Duarte</t>
+  </si>
+  <si>
+    <t>Conferente de Estoque</t>
+  </si>
+  <si>
+    <t>Gestao de Fornecedores</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>22/01/2025</t>
+  </si>
+  <si>
+    <t>Gestao de Residuos Industriais</t>
+  </si>
+  <si>
+    <t>Logistica de Producao</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Ana Costa</t>
+  </si>
+  <si>
+    <t>Supervisor de Producao</t>
+  </si>
+  <si>
+    <t>Gestao de Equipes</t>
+  </si>
+  <si>
+    <t>25/11/2027</t>
+  </si>
+  <si>
+    <t>Gestao de Projetos Industriais</t>
+  </si>
+  <si>
+    <t>26/01/2026</t>
+  </si>
+  <si>
+    <t>Seguranca Quimica</t>
+  </si>
+  <si>
+    <t>Beatriz Castro</t>
+  </si>
+  <si>
+    <t>Coordenador de Seguranca</t>
+  </si>
+  <si>
+    <t>Primeiros Socorros Industrial</t>
+  </si>
+  <si>
+    <t>05/02/2025</t>
+  </si>
+  <si>
+    <t>18/02/2025</t>
+  </si>
+  <si>
+    <t>Seguranca em Maquinas Industriais</t>
+  </si>
+  <si>
+    <t>04/07/2027</t>
+  </si>
+  <si>
+    <t>Bruno Carvalho</t>
+  </si>
+  <si>
+    <t>Supervisor de Qualidade</t>
+  </si>
+  <si>
+    <t>Auditoria Interna de Qualidade</t>
+  </si>
+  <si>
+    <t>Controle de Qualidade em Alimentos</t>
+  </si>
+  <si>
+    <t>05/10/2026</t>
+  </si>
+  <si>
+    <t>Legislacao Sanitaria</t>
+  </si>
+  <si>
+    <t>20/07/2027</t>
+  </si>
+  <si>
+    <t>Camila Ribeiro</t>
+  </si>
+  <si>
+    <t>Gerente de Producao</t>
+  </si>
+  <si>
+    <t>28/11/2024</t>
+  </si>
+  <si>
+    <t>09/04/2026</t>
+  </si>
+  <si>
+    <t>21/02/2025</t>
+  </si>
+  <si>
+    <t>Carlos Souza</t>
+  </si>
+  <si>
+    <t>Engenheiro de Alimentos</t>
+  </si>
+  <si>
+    <t>ISO 22000 - Seguranca de Alimentos</t>
+  </si>
+  <si>
+    <t>20/06/2025</t>
+  </si>
+  <si>
+    <t>Tecnologia de Processamento de Frutas</t>
+  </si>
+  <si>
+    <t>Diego Fernandes</t>
+  </si>
+  <si>
+    <t>Operador de Caldeira</t>
+  </si>
+  <si>
+    <t>Manutencao Preventiva Industrial</t>
+  </si>
+  <si>
+    <t>Fernanda Lima</t>
+  </si>
+  <si>
+    <t>Responsavel Tecnico</t>
+  </si>
+  <si>
+    <t>26/06/2027</t>
+  </si>
+  <si>
+    <t>29/01/2025</t>
+  </si>
+  <si>
+    <t>Gustavo Nunes</t>
+  </si>
+  <si>
+    <t>Nutricionista Industrial</t>
+  </si>
+  <si>
+    <t>04/01/2025</t>
+  </si>
+  <si>
+    <t>19/01/2026</t>
+  </si>
+  <si>
+    <t>Isabela Freitas</t>
+  </si>
+  <si>
+    <t>Assistente de RH</t>
+  </si>
+  <si>
+    <t>22/02/2025</t>
+  </si>
+  <si>
+    <t>Joao Silva</t>
+  </si>
+  <si>
+    <t>Operador de Maquinas</t>
+  </si>
+  <si>
+    <t>Boas Praticas de Fabricacao (BPF)</t>
+  </si>
+  <si>
+    <t>07/08/2025</t>
+  </si>
+  <si>
+    <t>Juliana Alves</t>
+  </si>
+  <si>
+    <t>Encarregado de Logistica</t>
+  </si>
+  <si>
+    <t>02/07/2027</t>
+  </si>
+  <si>
+    <t>Laura Martins</t>
+  </si>
+  <si>
+    <t>Eletricista Industrial</t>
+  </si>
+  <si>
+    <t>Eletricidade Industrial Basica</t>
+  </si>
+  <si>
+    <t>Lucas Santos</t>
+  </si>
+  <si>
+    <t>Analista de Qualidade</t>
+  </si>
+  <si>
+    <t>Analise Microbiologica</t>
+  </si>
+  <si>
+    <t>18/11/2025</t>
+  </si>
+  <si>
+    <t>19/12/2024</t>
+  </si>
+  <si>
+    <t>Calibracao de Equipamentos</t>
+  </si>
+  <si>
+    <t>22/11/2024</t>
+  </si>
+  <si>
+    <t>Marcos Torres</t>
+  </si>
+  <si>
+    <t>Auxiliar de Producao</t>
+  </si>
+  <si>
+    <t>21/12/2024</t>
+  </si>
+  <si>
+    <t>Higienizacao Industrial</t>
+  </si>
+  <si>
+    <t>Maria Oliveira</t>
+  </si>
+  <si>
+    <t>Tecnico de Laboratorio</t>
+  </si>
+  <si>
+    <t>16/10/2025</t>
+  </si>
+  <si>
+    <t>25/08/2027</t>
+  </si>
+  <si>
+    <t>29/01/2026</t>
+  </si>
+  <si>
+    <t>Patricia Mendes</t>
+  </si>
+  <si>
+    <t>Operador de Processos</t>
+  </si>
+  <si>
+    <t>Operacao de Empacotamento Automatizado</t>
+  </si>
+  <si>
+    <t>02/03/2025</t>
+  </si>
+  <si>
+    <t>18/12/2025</t>
+  </si>
+  <si>
+    <t>Pedro Rocha</t>
+  </si>
+  <si>
+    <t>Auxiliar de Limpeza</t>
+  </si>
+  <si>
+    <t>Rafael Pereira</t>
+  </si>
+  <si>
+    <t>Tecnico de Manutencao</t>
+  </si>
+  <si>
+    <t>17/11/2024</t>
+  </si>
+  <si>
+    <t>28/03/2025</t>
+  </si>
+  <si>
+    <t>Thiago Gomes</t>
+  </si>
+  <si>
+    <t>Operador de Empacotamento</t>
+  </si>
+  <si>
+    <t>27/11/2025</t>
+  </si>
+  <si>
+    <t>15/05/2025</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,25 +334,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <name val="Cambria"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -364,111 +349,89 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -476,12 +439,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -510,7 +473,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -531,7 +494,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -582,7 +545,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -600,35 +563,34 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.48"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="38.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.77"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -645,7 +607,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -659,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -679,7 +641,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -693,7 +655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,7 +672,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -724,7 +686,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -741,7 +703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>13</v>
       </c>
@@ -755,7 +717,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -772,7 +734,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -789,7 +751,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -806,7 +768,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -820,7 +782,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -837,7 +799,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -854,7 +816,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
@@ -868,7 +830,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -885,7 +847,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
@@ -902,7 +864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -919,7 +881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>39</v>
       </c>
@@ -933,7 +895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>39</v>
       </c>
@@ -947,7 +909,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
@@ -964,7 +926,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>39</v>
       </c>
@@ -978,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -992,7 +954,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>44</v>
       </c>
@@ -1006,7 +968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1020,7 +982,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>47</v>
       </c>
@@ -1034,7 +996,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1051,7 +1013,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -1068,7 +1030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>47</v>
       </c>
@@ -1082,7 +1044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1096,7 +1058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
@@ -1113,7 +1075,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>51</v>
       </c>
@@ -1130,7 +1092,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
@@ -1144,7 +1106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>55</v>
       </c>
@@ -1158,7 +1120,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>55</v>
       </c>
@@ -1175,7 +1137,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>58</v>
       </c>
@@ -1189,7 +1151,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>58</v>
       </c>
@@ -1206,7 +1168,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>58</v>
       </c>
@@ -1220,7 +1182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>58</v>
       </c>
@@ -1234,7 +1196,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>62</v>
       </c>
@@ -1248,7 +1210,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>62</v>
       </c>
@@ -1265,7 +1227,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>62</v>
       </c>
@@ -1279,7 +1241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -1293,7 +1255,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>65</v>
       </c>
@@ -1307,7 +1269,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>65</v>
       </c>
@@ -1321,7 +1283,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>68</v>
       </c>
@@ -1338,7 +1300,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>68</v>
       </c>
@@ -1355,7 +1317,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>68</v>
       </c>
@@ -1369,7 +1331,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>68</v>
       </c>
@@ -1386,7 +1348,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>75</v>
       </c>
@@ -1403,7 +1365,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>75</v>
       </c>
@@ -1417,7 +1379,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>75</v>
       </c>
@@ -1431,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>79</v>
       </c>
@@ -1448,7 +1410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>79</v>
       </c>
@@ -1465,7 +1427,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>79</v>
       </c>
@@ -1479,7 +1441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>79</v>
       </c>
@@ -1496,7 +1458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>84</v>
       </c>
@@ -1513,7 +1475,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>84</v>
       </c>
@@ -1527,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>84</v>
       </c>
@@ -1544,7 +1506,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>89</v>
       </c>
@@ -1558,7 +1520,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -1572,7 +1534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>89</v>
       </c>
@@ -1586,7 +1548,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>91</v>
       </c>
@@ -1603,7 +1565,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>91</v>
       </c>
@@ -1617,7 +1579,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>91</v>
       </c>
@@ -1634,7 +1596,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
@@ -1648,7 +1610,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>95</v>
       </c>
@@ -1665,7 +1627,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>95</v>
       </c>
@@ -1683,12 +1645,7 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>